<commit_message>
add driver property to families, and option to search by driver
</commit_message>
<xml_diff>
--- a/backend/נתמכים.xlsx
+++ b/backend/נתמכים.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\shalom\Gmah\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82FCF3D-2DEA-4A6C-8FBC-BD5ED0802422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2E79ED-D0A9-4183-BCCC-92E6EF343970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>שם מלא</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t>נחום</t>
+  </si>
+  <si>
+    <t>נהג</t>
+  </si>
+  <si>
+    <t>פלוני</t>
   </si>
 </sst>
 </file>
@@ -256,12 +262,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="נתמכים" displayName="נתמכים" ref="A1:J2" headerRowDxfId="1" tableBorderDxfId="0" dataCellStyle="שורת נתמך">
-  <autoFilter ref="A1:J2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J2">
-    <sortCondition ref="I1:I2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="נתמכים" displayName="נתמכים" ref="A1:K2" headerRowDxfId="1" tableBorderDxfId="0" dataCellStyle="שורת נתמך">
+  <autoFilter ref="A1:K2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K2">
+    <sortCondition ref="J1:J2"/>
   </sortState>
-  <tableColumns count="10">
+  <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="שם מלא" totalsRowLabel="סה&quot;כ" dataCellStyle="שורת נתמך"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="רחוב" dataCellStyle="שורת נתמך"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="בניין" dataCellStyle="שורת נתמך"/>
@@ -269,6 +275,7 @@
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="קומה" dataCellStyle="שורת נתמך"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="מס' בית" dataCellStyle="שורת נתמך"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="מס' פלאפון" dataCellStyle="שורת נתמך"/>
+    <tableColumn id="10" xr3:uid="{D6A2570F-6BEC-475E-8659-B642D346D4A3}" name="נהג" dataCellStyle="שורת נתמך"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="נהג במקור" dataCellStyle="שורת נתמך"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="ממליץ" dataCellStyle="שורת נתמך"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="הערות" totalsRowFunction="count" dataCellStyle="שורת נתמך"/>
@@ -574,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -587,17 +594,18 @@
     <col min="3" max="5" width="8.796875" style="4" customWidth="1"/>
     <col min="6" max="6" width="11" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.3984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.796875" style="4" customWidth="1"/>
-    <col min="12" max="12" width="12.69921875" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.19921875" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="25" width="8.796875" style="4" customWidth="1"/>
-    <col min="26" max="16384" width="8.796875" style="4"/>
+    <col min="8" max="8" width="11.5" style="4" customWidth="1"/>
+    <col min="9" max="9" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.3984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.796875" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.69921875" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.19921875" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="26" width="8.796875" style="4" customWidth="1"/>
+    <col min="27" max="16384" width="8.796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -620,16 +628,19 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -650,10 +661,13 @@
         <v>12</v>
       </c>
       <c r="H2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="5"/>
       <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add named style instead of throwing error if its not there
</commit_message>
<xml_diff>
--- a/backend/נתמכים.xlsx
+++ b/backend/נתמכים.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\shalom\Gmah\backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\shalom\gmah\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2E79ED-D0A9-4183-BCCC-92E6EF343970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53B5BF6-FD52-4F5F-B340-AD1F49F440A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="נתמכים" sheetId="1" r:id="rId1"/>
@@ -43,6 +43,9 @@
     <t>מס' פלאפון</t>
   </si>
   <si>
+    <t>נהג</t>
+  </si>
+  <si>
     <t>נהג במקור</t>
   </si>
   <si>
@@ -61,13 +64,10 @@
     <t>054-4751400</t>
   </si>
   <si>
+    <t>פלוני</t>
+  </si>
+  <si>
     <t>נחום</t>
-  </si>
-  <si>
-    <t>נהג</t>
-  </si>
-  <si>
-    <t>פלוני</t>
   </si>
 </sst>
 </file>
@@ -78,7 +78,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -97,23 +97,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -149,43 +141,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="1"/>
+      <left style="medium">
+        <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color theme="1"/>
+      <right style="medium">
+        <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color theme="1"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color theme="1"/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -275,7 +267,7 @@
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="קומה" dataCellStyle="שורת נתמך"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="מס' בית" dataCellStyle="שורת נתמך"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="מס' פלאפון" dataCellStyle="שורת נתמך"/>
-    <tableColumn id="10" xr3:uid="{D6A2570F-6BEC-475E-8659-B642D346D4A3}" name="נהג" dataCellStyle="שורת נתמך"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="נהג" dataCellStyle="שורת נתמך"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="נהג במקור" dataCellStyle="שורת נתמך"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="ממליץ" dataCellStyle="שורת נתמך"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="הערות" totalsRowFunction="count" dataCellStyle="שורת נתמך"/>
@@ -584,28 +576,28 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7890625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.19921875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="8.796875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="16.20703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.47265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="8.7890625" style="4" customWidth="1"/>
     <col min="6" max="6" width="11" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5" style="4" customWidth="1"/>
+    <col min="7" max="7" width="11.47265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.47265625" style="4" customWidth="1"/>
     <col min="9" max="9" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.3984375" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.796875" style="4" customWidth="1"/>
-    <col min="13" max="13" width="12.69921875" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.19921875" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="26" width="8.796875" style="4" customWidth="1"/>
-    <col min="27" max="16384" width="8.796875" style="4"/>
+    <col min="10" max="10" width="15.41796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7890625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7890625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.68359375" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.20703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="27" width="8.7890625" style="4" customWidth="1"/>
+    <col min="28" max="16384" width="8.7890625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -628,24 +620,24 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="5">
         <v>10</v>
@@ -658,13 +650,13 @@
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>

</xml_diff>